<commit_message>
[Avada] menual update - 설치 방법
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="login" sheetId="2" r:id="rId1"/>
+    <sheet name="Avada 설치" sheetId="4" r:id="rId2"/>
+    <sheet name="basic Inform" sheetId="1" r:id="rId3"/>
+    <sheet name="Plug-in" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'basic Inform'!$A$1:$M$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Plug-in'!$A$1:$M$78</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -27,6 +33,226 @@
   </si>
   <si>
     <t>Layout 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guncom1.cafe24.com/wp-admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://theme-fusion.com/support/documentation/avada-documentation/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_execution_time 180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memory_limit 128M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recommended PHP Configuration Limits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_max_size 32M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload_max_filesize 32M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada menu의 System Status에서 필요한 사양을 확인 할 수 있으며, 문제가 되는 항목은 Red Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로 표시되며, 변경 방법에 대한 link도 제공된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. WordPress Reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WordPress 초기 설정으로 원복해 주는 plug-in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada dome theme 삭제 및 변경시 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wordpress.org/plugins/wordpress-reset/#description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플러그인을 비활성화하고 모든 페이지, 게시물, 메뉴, 슬라이더, 위젯 데이터, 퓨전 테마 옵션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등을 제거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Admin Side bar menu의 도구에 등록됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) text box에 reset을 입력하고, Reset 버튼 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ wordpress가 영문으로 설정되므로, admin side bar menu의 설정에서 언어를 한국어로 변경한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fusion Patcher 상태 원복됨.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada의 System 설정 상태는 유지됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Registration에서 token 재입력 해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slider Revolution과 Layer Slider는 Avada token 등록 후 사용 가능함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://themeforest.net/page/top_sellers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. themeforest에서 테마 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 구매 후 메뉴 상단의 ID 드롭다운 menu의 Download를 선택하면 아래와 같은 화면이 나옴.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Download 버튼을 선택하고, All files &amp; documentation을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.Download된 압축 파일을 풀어준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Themes 폴더에 아바다 테마와 차일드 테마가 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. WP 외모에서 본테마를 설치 후 비활성화 상태로 둔다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. WP 외모에서 차일드 테마를 설치 후 활성화 시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">테마의 파일을 수정,변경시 차일드 테마를 사용하며, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추후 테마가 upgrade되더라도 차일드 테마의 수정 사항은 유지가 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 제품등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테마 설치 후, WP side bar menu에 Avada menu가 생성되며, 이를 선택하고 Registration을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하단의 Generate A Personal Token link를 선택하여, envateAPI create a token 페이지로 이동한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래의 항목들을 입력 및 선택 후 create Token을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Token name : 사용자가 임의로 이름 명시 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Permissions needed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View Your Envato Account Username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download Your Purchased Items</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List Purchases You’ve Made</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verify Purchases You've Made</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>therms and conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정상적으로 처리시 Success 와 함께 token이 생성된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성된 token을 copy하여 WP의 Registration에 입력 후 submit 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. System Status 체크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">WP side-bar menu에서 Plugins을 선택하면, Avada에서 제공되는 Plugin이 list-up되며, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이를 모두 설치한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Avada에서 제공하는 Plug-In 설치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada가 최적화 해 놓은 Plugin이므로, 동일 기능의 Plugin인 경우에는 Avada에서 제공하는 plugin을 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. 테마 patch 하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP side-bar menu에서 Fusion Patcher를 선택하고, 순서에 맞춰 Patch 실행함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. WP의 알림판 &gt; 업데이트 메뉴에서 theme와 Plugin을 update한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada 설치 방법</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -34,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +281,71 @@
       <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -79,9 +370,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -93,6 +392,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -102,15 +404,472 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>71367</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>82135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>113783</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>549108</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>198783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="626302" y="1117461"/>
+          <a:ext cx="5753763" cy="3015561"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57979</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>530087</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>17269</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="그룹 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="612914" y="4588565"/>
+          <a:ext cx="5748130" cy="1433595"/>
+          <a:chOff x="612914" y="4588565"/>
+          <a:chExt cx="5748130" cy="1433595"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="612914" y="4588565"/>
+            <a:ext cx="5748130" cy="1433595"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3801717" y="5035826"/>
+            <a:ext cx="1143000" cy="231913"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>74544</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>173491</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="그룹 10"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="629479" y="8158370"/>
+          <a:ext cx="5789543" cy="2782512"/>
+          <a:chOff x="629479" y="8158370"/>
+          <a:chExt cx="5789543" cy="2782512"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="그림 6"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="629479" y="8158370"/>
+            <a:ext cx="5789543" cy="2782512"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2103784" y="9243391"/>
+            <a:ext cx="637759" cy="248479"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>24850</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>596347</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>4043</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="그룹 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="579785" y="13914783"/>
+          <a:ext cx="5847519" cy="1412086"/>
+          <a:chOff x="579785" y="13914783"/>
+          <a:chExt cx="5847519" cy="1412086"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8" name="그림 7"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="579785" y="13914783"/>
+            <a:ext cx="5847519" cy="1412086"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5486400" y="14357074"/>
+            <a:ext cx="849796" cy="245165"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>91110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>612913</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>148705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="그림 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="646044" y="17484588"/>
+          <a:ext cx="5797826" cy="2128247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>84896</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>109332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>584751</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146914</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -134,8 +893,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="962025" y="1123951"/>
-          <a:ext cx="5267325" cy="3809482"/>
+          <a:off x="772353" y="8184875"/>
+          <a:ext cx="5278920" cy="3764756"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -152,6 +911,339 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>629478</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165973</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="571500" y="1308652"/>
+          <a:ext cx="4861891" cy="2170364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>413468</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>115955</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="그룹 8"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1043609" y="5433393"/>
+          <a:ext cx="1332837" cy="1308649"/>
+          <a:chOff x="886240" y="4605131"/>
+          <a:chExt cx="1332836" cy="1308651"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="그림 6"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="886240" y="4605131"/>
+            <a:ext cx="1332836" cy="1308651"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="894522" y="5623891"/>
+            <a:ext cx="861392" cy="231913"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>41414</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>49694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>339588</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>87784</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="그룹 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1043610" y="7296977"/>
+          <a:ext cx="4696239" cy="2729937"/>
+          <a:chOff x="1880153" y="5996608"/>
+          <a:chExt cx="4696239" cy="2729937"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="그림 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1880153" y="5996608"/>
+            <a:ext cx="4696239" cy="2729937"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1954695" y="7827066"/>
+            <a:ext cx="1118153" cy="273325"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1958009" y="8219663"/>
+            <a:ext cx="626166" cy="245164"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -200,7 +1292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,7 +1327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,66 +1536,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>2</v>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId2"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.25" style="2" customWidth="1"/>
+    <col min="2" max="3" width="3" style="6" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C54" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C55" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D56" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C63" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C64" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C66" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="2"/>
+      <c r="C71"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" s="2"/>
+      <c r="C74"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B75" s="2"/>
+      <c r="C75"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B76" s="2"/>
+      <c r="C76" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B77" s="2"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B78" s="2"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B79" s="3"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B80" s="3"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="3"/>
+      <c r="C82" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="7"/>
+      <c r="C83" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="7"/>
+      <c r="C84" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="7"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="7"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="7"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="37" max="11" man="1"/>
+  </rowBreaks>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="2.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.625" customWidth="1"/>
+    <col min="4" max="4" width="3.75" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M35"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.375" customWidth="1"/>
+    <col min="2" max="2" width="3.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="3.625" style="6" customWidth="1"/>
+    <col min="6" max="13" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="7"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" location="description"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Avada] menual update - Layout 설정 방법
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
     <sheet name="Avada 설치" sheetId="4" r:id="rId2"/>
     <sheet name="basic Inform" sheetId="1" r:id="rId3"/>
     <sheet name="Plug-in" sheetId="3" r:id="rId4"/>
+    <sheet name="Layout" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'basic Inform'!$A$1:$M$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Plug-in'!$A$1:$M$78</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,6 +254,14 @@
   </si>
   <si>
     <t>Avada 설치 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. sidebar menu 생성 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fusion Builder -&gt; Library -&gt; Demos -&gt; Sidebar Page  참조</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1249,6 +1258,66 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="657225" y="1000125"/>
+          <a:ext cx="8029575" cy="4495800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -1292,7 +1361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1327,7 +1396,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1833,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1885,7 +1954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M35"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -1980,4 +2049,35 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="4.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Avada] option menu 추가
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -12,18 +12,20 @@
     <sheet name="basic Inform" sheetId="1" r:id="rId3"/>
     <sheet name="Plug-in" sheetId="3" r:id="rId4"/>
     <sheet name="Layout" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'basic Inform'!$A$1:$M$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Plug-in'!$A$1:$M$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Sheet1!$A$1:$Q$273</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,6 +264,78 @@
   </si>
   <si>
     <t>Fusion Builder -&gt; Library -&gt; Demos -&gt; Sidebar Page  참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Header 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Header Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header의 위치와 Header content의 디자인 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top - 7가지 디자인이 있으며, 선택된 디자인에 따른 content를 선택할 수 있다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">슬라이더 설정이 가능한 layout 이며, Header 위/아래 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left/Right - 한가지 형태이며, Main menu이외의 3개의 content 추가가 가능한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) Header Background Image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역에 Background image 설정, image 선택이 없는 경우 background color가 설정됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3) Header Styling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역의 Padding(여백) 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역 그림자 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo와 Menu 배치를 폭 100%로 사용 - Logo는 좌측, Menu는 우측으로 정렬됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Background color 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sticky Header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역에 scroll을 내려도 상단에 유지되도록 하는 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1318,6 +1392,1272 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647701</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165753</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="895351" y="895350"/>
+          <a:ext cx="6762750" cy="2832753"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>55419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1447801" y="4676775"/>
+          <a:ext cx="4610099" cy="3551094"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>153786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1476376" y="8429625"/>
+          <a:ext cx="6457950" cy="2620761"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47627</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>200285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1981202" y="16821151"/>
+          <a:ext cx="4981574" cy="2238634"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>46754</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="그림 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1390650" y="11382376"/>
+          <a:ext cx="6172200" cy="5218828"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>184448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="그림 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1990725" y="19345276"/>
+          <a:ext cx="5019675" cy="2632372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>541244</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="그림 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="895350" y="22679025"/>
+          <a:ext cx="7342094" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>204697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="그림 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="933450" y="23622000"/>
+          <a:ext cx="7229475" cy="4033747"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>5964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="그림 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1133476" y="28279725"/>
+          <a:ext cx="7010400" cy="1482339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="그림 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1190625" y="30222825"/>
+          <a:ext cx="4953000" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>207750</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="28" name="그룹 27"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1206314" y="31653816"/>
+          <a:ext cx="7027209" cy="916522"/>
+          <a:chOff x="1190625" y="31156275"/>
+          <a:chExt cx="7381875" cy="948351"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="그림 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1209675" y="31156275"/>
+            <a:ext cx="7362825" cy="948351"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="27" name="모서리가 둥근 직사각형 26"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1190625" y="31661100"/>
+            <a:ext cx="7381875" cy="209550"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>46136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="그림 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1143000" y="34585276"/>
+          <a:ext cx="7058025" cy="874810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="그림 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1143000" y="33604200"/>
+          <a:ext cx="4991100" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="그림 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="35928300"/>
+          <a:ext cx="5200650" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>612937</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="그림 35"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="37347526"/>
+          <a:ext cx="7137562" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>170794</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="43" name="그룹 42"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1177738" y="39417252"/>
+          <a:ext cx="7065309" cy="4826277"/>
+          <a:chOff x="1162050" y="38795326"/>
+          <a:chExt cx="7067550" cy="4752318"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="38" name="그림 37"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1162050" y="38795326"/>
+            <a:ext cx="7067550" cy="4752318"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="TextBox 38"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5924550" y="39652575"/>
+            <a:ext cx="1205843" cy="336246"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>PC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>에서의 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>On/Off</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="TextBox 39"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5895975" y="40433625"/>
+            <a:ext cx="1479316" cy="336246"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>테블렛에서의 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>On/Off</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="41" name="TextBox 40"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5905500" y="41233725"/>
+            <a:ext cx="1479316" cy="336246"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>모바일에서의 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>On/Off</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="42" name="TextBox 41"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5867400" y="43062525"/>
+            <a:ext cx="1793889" cy="336246"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Sticky </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>상태에서의 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>BG color</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>42887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="그림 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="44729400"/>
+          <a:ext cx="7115175" cy="995387"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -1361,7 +2701,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1396,7 +2736,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1628,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E98"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A88" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2055,8 +3395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2080,4 +3420,118 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F185"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A183" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="W204" sqref="W204"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="3.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F81" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C134" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D171" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="184" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D184" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="185" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E185" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="71" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Avada] Logo menu 추가
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -4,28 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="2" r:id="rId1"/>
+    <sheet name="basic Inform" sheetId="1" r:id="rId1"/>
     <sheet name="Avada 설치" sheetId="4" r:id="rId2"/>
-    <sheet name="basic Inform" sheetId="1" r:id="rId3"/>
-    <sheet name="Plug-in" sheetId="3" r:id="rId4"/>
-    <sheet name="Layout" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Plug-in" sheetId="3" r:id="rId3"/>
+    <sheet name="Layout" sheetId="5" r:id="rId4"/>
+    <sheet name="Header" sheetId="6" r:id="rId5"/>
+    <sheet name="Logo" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'basic Inform'!$A$1:$M$58</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Plug-in'!$A$1:$M$78</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Sheet1!$A$1:$Q$273</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'basic Inform'!$A$1:$M$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Header!$A$1:$Q$212</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Logo!$A$1:$P$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Plug-in'!$A$1:$M$67</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -336,6 +337,50 @@
   </si>
   <si>
     <t>Header 영역에 scroll을 내려도 상단에 유지되도록 하는 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Logo 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Alignment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header내의 Logo 위치 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 5에서만 사용 가능 - Header layout menu에서 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Margins</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo의 4방향에 대한 margin 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Background</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo의 background color 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -483,6 +528,66 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>84896</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>109332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>584751</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146914</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="772353" y="8184875"/>
+          <a:ext cx="5278920" cy="3764756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -918,66 +1023,6 @@
         <a:xfrm>
           <a:off x="646044" y="17484588"/>
           <a:ext cx="5797826" cy="2128247"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>84896</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>109332</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>584751</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>146914</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="772353" y="8184875"/>
-          <a:ext cx="5278920" cy="3764756"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1964,8 +2009,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1206314" y="31653816"/>
-          <a:ext cx="7027209" cy="916522"/>
+          <a:off x="1190626" y="31156275"/>
+          <a:ext cx="7029450" cy="903075"/>
           <a:chOff x="1190625" y="31156275"/>
           <a:chExt cx="7381875" cy="948351"/>
         </a:xfrm>
@@ -2288,9 +2333,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>207</xdr:row>
-      <xdr:rowOff>170794</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>162583</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2299,8 +2344,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1177738" y="39417252"/>
-          <a:ext cx="7065309" cy="4826277"/>
+          <a:off x="1162050" y="38795326"/>
+          <a:ext cx="6743700" cy="4534557"/>
           <a:chOff x="1162050" y="38795326"/>
           <a:chExt cx="7067550" cy="4752318"/>
         </a:xfrm>
@@ -2603,15 +2648,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>213</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>42887</xdr:rowOff>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>181815</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2635,8 +2680,228 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1171575" y="44729400"/>
-          <a:ext cx="7115175" cy="995387"/>
+          <a:off x="1152526" y="43472101"/>
+          <a:ext cx="6610350" cy="924764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="직선 화살표 연결선 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4219575" y="43205400"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>67953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="590550" y="266700"/>
+          <a:ext cx="7400925" cy="3573153"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>17671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1143000" y="4667250"/>
+          <a:ext cx="6734175" cy="589171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>201428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1133475" y="5695950"/>
+          <a:ext cx="6791325" cy="582428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2945,22 +3210,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
+  <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="2.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.625" customWidth="1"/>
+    <col min="4" max="4" width="3.75" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2968,14 +3269,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E98"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A88" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A79" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.25" style="2" customWidth="1"/>
-    <col min="2" max="3" width="3" style="6" customWidth="1"/>
+    <col min="2" max="2" width="3" style="9" customWidth="1"/>
+    <col min="3" max="3" width="3" style="6" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2985,7 +3287,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2995,17 +3297,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3015,12 +3317,12 @@
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3035,7 +3337,7 @@
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3100,7 +3402,7 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3154,63 +3456,43 @@
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B79" s="3"/>
+      <c r="B79" s="2"/>
       <c r="C79" s="9"/>
       <c r="D79" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B80" s="3"/>
+      <c r="B80" s="2"/>
       <c r="C80" s="9"/>
       <c r="D80" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C81"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="3"/>
+      <c r="B82" s="2"/>
       <c r="C82" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="7"/>
       <c r="C83" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="7"/>
       <c r="C84" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="7"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="7"/>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="7"/>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="7"/>
-    </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3220,7 +3502,7 @@
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3239,58 +3521,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C39"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="2.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.625" customWidth="1"/>
-    <col min="4" max="4" width="3.75" customWidth="1"/>
-    <col min="5" max="5" width="4.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M35"/>
   <sheetViews>
@@ -3387,11 +3617,14 @@
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="24" max="12" man="1"/>
+  </rowBreaks>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C3"/>
   <sheetViews>
@@ -3422,41 +3655,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A183" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="W204" sqref="W204"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="3.625" customWidth="1"/>
+    <col min="1" max="2" width="3.625" customWidth="1"/>
+    <col min="3" max="5" width="3.625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3466,7 +3701,7 @@
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3481,47 +3716,47 @@
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C107" t="s">
+      <c r="C107" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
+      <c r="D108" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C134" t="s">
+      <c r="C134" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D135" t="s">
+      <c r="D135" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="144" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D144" t="s">
+      <c r="D144" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D160" t="s">
+      <c r="D160" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D171" t="s">
+      <c r="D171" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="184" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D184" t="s">
+      <c r="D184" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="185" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E185" t="s">
+      <c r="E185" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3534,4 +3769,85 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E39"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
+    <col min="2" max="4" width="3.625" style="2" customWidth="1"/>
+    <col min="5" max="7" width="3.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="16" max="47" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Avada] class shop demo setup #1
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="basic Inform" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,15 @@
     <sheet name="Layout" sheetId="5" r:id="rId4"/>
     <sheet name="Header" sheetId="6" r:id="rId5"/>
     <sheet name="Logo" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'basic Inform'!$A$1:$M$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Header!$A$1:$Q$212</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Logo!$A$1:$P$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Sheet1!$A$1:$Q$196</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'WP Reset'!$A$1:$M$67</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -405,6 +408,110 @@
   </si>
   <si>
     <t>QnA - 게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>템플릿을 기존으로 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar menu가 있는 경우, 100% Width는 설정이 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Side Navi..의 경우, 아래와 같이 메뉴가 하나 더 들어감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebars를 Products Sidebar로 설정 - 포함되는 메뉴는 위젯에서 변경 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heakder Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content option 4 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main menu 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Option - Main menu 높이와 Highlight style 및 color를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Option - Menu 정렬 방식 및 Hover color를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외모 &gt; Main menu - Sticky 설정을 위해 아래와 같이 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer widget을 사용하지 않는 경우, OFF로 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer widget이 ON되어 있는 상태이며, 목록은 위젯의 Footer Widget 1,2,3,4에서 선택할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar 위젯 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위젯의 Products Sidebar에 woocommerce의 categories를 추가하고, 기존 설정을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product page의 Sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; Woocommerce Products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home을 제외한 모든 Page에 sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; Pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar menu 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home은 Page내에 별개의 설정이 필요함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option의 Sidebar의 Pages 설정은 적용되지 않음 - 원인 분석 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product Archive의 Sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; WooCommerce Archive</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,7 +519,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +607,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -522,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -533,6 +649,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2947,6 +3064,1168 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>62534</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>51353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>14827</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>157370</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4883012" y="465483"/>
+          <a:ext cx="2014663" cy="2176669"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>65846</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>496956</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>174158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="985216" y="1101587"/>
+          <a:ext cx="2269849" cy="1557353"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>98977</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>121339</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>536415</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>83238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="711890" y="13994709"/>
+          <a:ext cx="7394829" cy="2653747"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66260</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>641074</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="985630" y="7272130"/>
+          <a:ext cx="4475922" cy="1009236"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>115958</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161165</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="728871" y="9160566"/>
+          <a:ext cx="4252772" cy="2252869"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>173934</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>575665</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>107676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="그림 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="786847" y="11918674"/>
+          <a:ext cx="4609296" cy="2269436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>231915</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>397567</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>146571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="그림 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="844828" y="14784456"/>
+          <a:ext cx="5748130" cy="1513201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107674</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>60377</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="720587" y="17426608"/>
+          <a:ext cx="7230717" cy="2304964"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>273326</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>124240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>339587</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>104332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="그림 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8531087" y="21037827"/>
+          <a:ext cx="4878457" cy="1429548"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>135261</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>670892</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>150553</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="그림 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1054631" y="20201282"/>
+          <a:ext cx="5811652" cy="3347640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>364435</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>194263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="그림 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="960783" y="24880957"/>
+          <a:ext cx="2849217" cy="2852980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>99390</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>49697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>289892</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>194014</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="그림 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1018760" y="24897523"/>
+          <a:ext cx="5466523" cy="3457361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>74543</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>289892</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>93427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="그림 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="993913" y="21170348"/>
+          <a:ext cx="5491370" cy="3149710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>41414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>629480</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>134857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="그림 34"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="927653" y="29237610"/>
+          <a:ext cx="5897218" cy="2164095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>120098</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>279124</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>30251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3549098" y="349943"/>
+          <a:ext cx="7702826" cy="4080858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>655942</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>173107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="209550"/>
+          <a:ext cx="2027542" cy="3735457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="직선 화살표 연결선 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2000250" y="2133600"/>
+          <a:ext cx="2171700" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="직선 화살표 연결선 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="895351"/>
+          <a:ext cx="3295650" cy="600074"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4781550" y="1285875"/>
+          <a:ext cx="5172075" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="직선 화살표 연결선 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1552575" y="895350"/>
+          <a:ext cx="2000250" cy="752476"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762375" y="352425"/>
+          <a:ext cx="7486650" cy="1323975"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -2990,7 +4269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3025,7 +4304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3236,7 +4515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -3711,8 +4990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F185"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B124" sqref="B1:B1048576"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A187" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3902,4 +5181,177 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D169"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A136" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="Q149" sqref="Q149"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="4" style="2" customWidth="1"/>
+    <col min="3" max="9" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D84" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C101" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C102" s="2"/>
+      <c r="D102" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C103" s="2"/>
+      <c r="D103" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C120" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C121" s="2"/>
+      <c r="D121" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C140" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C141" s="2"/>
+      <c r="D141" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B155" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C169" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Avada] classic shop demo setup #2
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="basic Inform" sheetId="1" r:id="rId1"/>
@@ -14,22 +14,480 @@
     <sheet name="Header" sheetId="6" r:id="rId5"/>
     <sheet name="Logo" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
+    <sheet name="상품page" sheetId="11" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Avada 설치'!$A$1:$L$123</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'basic Inform'!$A$1:$M$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Header!$A$1:$Q$212</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Logo!$A$1:$P$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">Sheet1!$A$1:$Q$196</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Sheet1!$A$1:$Q$142</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'WP Reset'!$A$1:$M$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">상품page!$A$1:$Q$96</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+  <si>
+    <t>max_execution_time 180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memory_limit 128M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recommended PHP Configuration Limits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_max_size 32M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload_max_filesize 32M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada menu의 System Status에서 필요한 사양을 확인 할 수 있으며, 문제가 되는 항목은 Red Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로 표시되며, 변경 방법에 대한 link도 제공된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. WordPress Reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WordPress 초기 설정으로 원복해 주는 plug-in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada dome theme 삭제 및 변경시 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wordpress.org/plugins/wordpress-reset/#description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플러그인을 비활성화하고 모든 페이지, 게시물, 메뉴, 슬라이더, 위젯 데이터, 퓨전 테마 옵션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등을 제거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Admin Side bar menu의 도구에 등록됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) text box에 reset을 입력하고, Reset 버튼 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ wordpress가 영문으로 설정되므로, admin side bar menu의 설정에서 언어를 한국어로 변경한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fusion Patcher 상태 원복됨.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada의 System 설정 상태는 유지됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Registration에서 token 재입력 해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slider Revolution과 Layer Slider는 Avada token 등록 후 사용 가능함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://themeforest.net/page/top_sellers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. themeforest에서 테마 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 구매 후 메뉴 상단의 ID 드롭다운 menu의 Download를 선택하면 아래와 같은 화면이 나옴.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Download 버튼을 선택하고, All files &amp; documentation을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.Download된 압축 파일을 풀어준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Themes 폴더에 아바다 테마와 차일드 테마가 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. WP 외모에서 본테마를 설치 후 비활성화 상태로 둔다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. WP 외모에서 차일드 테마를 설치 후 활성화 시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">테마의 파일을 수정,변경시 차일드 테마를 사용하며, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추후 테마가 upgrade되더라도 차일드 테마의 수정 사항은 유지가 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 제품등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테마 설치 후, WP side bar menu에 Avada menu가 생성되며, 이를 선택하고 Registration을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하단의 Generate A Personal Token link를 선택하여, envateAPI create a token 페이지로 이동한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래의 항목들을 입력 및 선택 후 create Token을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Token name : 사용자가 임의로 이름 명시 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Permissions needed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View Your Envato Account Username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download Your Purchased Items</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List Purchases You’ve Made</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verify Purchases You've Made</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>therms and conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정상적으로 처리시 Success 와 함께 token이 생성된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성된 token을 copy하여 WP의 Registration에 입력 후 submit 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. System Status 체크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">WP side-bar menu에서 Plugins을 선택하면, Avada에서 제공되는 Plugin이 list-up되며, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이를 모두 설치한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Avada에서 제공하는 Plug-In 설치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada가 최적화 해 놓은 Plugin이므로, 동일 기능의 Plugin인 경우에는 Avada에서 제공하는 plugin을 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. 테마 patch 하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP side-bar menu에서 Fusion Patcher를 선택하고, 순서에 맞춰 Patch 실행함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. WP의 알림판 &gt; 업데이트 메뉴에서 theme와 Plugin을 update한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada 설치 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. sidebar menu 생성 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fusion Builder -&gt; Library -&gt; Demos -&gt; Sidebar Page  참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Header 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Header Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header의 위치와 Header content의 디자인 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top - 7가지 디자인이 있으며, 선택된 디자인에 따른 content를 선택할 수 있다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">슬라이더 설정이 가능한 layout 이며, Header 위/아래 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left/Right - 한가지 형태이며, Main menu이외의 3개의 content 추가가 가능한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) Header Background Image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역에 Background image 설정, image 선택이 없는 경우 background color가 설정됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3) Header Styling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역의 Padding(여백) 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역 그림자 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo와 Menu 배치를 폭 100%로 사용 - Logo는 좌측, Menu는 우측으로 정렬됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Background color 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sticky Header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 영역에 scroll을 내려도 상단에 유지되도록 하는 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Logo 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Alignment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header내의 Logo 위치 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 5에서만 사용 가능 - Header layout menu에서 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Margins</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo의 4방향에 대한 margin 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo Background</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logo의 background color 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lAPnrqeAhAPp0mygCH27vMuMA9XOfIjx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메뉴  한글화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송장출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마일리지 적립</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QnA - 게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>템플릿을 기존으로 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar menu가 있는 경우, 100% Width는 설정이 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Side Navi..의 경우, 아래와 같이 메뉴가 하나 더 들어감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebars를 Products Sidebar로 설정 - 포함되는 메뉴는 위젯에서 변경 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heakder Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content option 4 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main menu 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Option - Main menu 높이와 Highlight style 및 color를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Option - Menu 정렬 방식 및 Hover color를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외모 &gt; Main menu - Sticky 설정을 위해 아래와 같이 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer widget을 사용하지 않는 경우, OFF로 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer widget이 ON되어 있는 상태이며, 목록은 위젯의 Footer Widget 1,2,3,4에서 선택할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar 위젯 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위젯의 Products Sidebar에 woocommerce의 categories를 추가하고, 기존 설정을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product page의 Sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; Woocommerce Products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; Pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home은 Page내에 별개의 설정이 필요함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product Archive의 Sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option &gt; Sidebars &gt; WooCommerce Archive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guncom1.cafe24.com/wp-admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Avada 참조 site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,479 +497,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Layout 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>guncom1.cafe24.com/wp-admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://theme-fusion.com/support/documentation/avada-documentation/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>max_execution_time 180</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memory_limit 128M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recommended PHP Configuration Limits</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post_max_size 32M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>upload_max_filesize 32M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada menu의 System Status에서 필요한 사양을 확인 할 수 있으며, 문제가 되는 항목은 Red Text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로 표시되며, 변경 방법에 대한 link도 제공된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. WordPress Reset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WordPress 초기 설정으로 원복해 주는 plug-in</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada dome theme 삭제 및 변경시 사용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://wordpress.org/plugins/wordpress-reset/#description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플러그인을 비활성화하고 모든 페이지, 게시물, 메뉴, 슬라이더, 위젯 데이터, 퓨전 테마 옵션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>등을 제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1) Admin Side bar menu의 도구에 등록됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2) text box에 reset을 입력하고, Reset 버튼 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>※ wordpress가 영문으로 설정되므로, admin side bar menu의 설정에서 언어를 한국어로 변경한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fusion Patcher 상태 원복됨.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada의 System 설정 상태는 유지됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada Registration에서 token 재입력 해야 함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slider Revolution과 Layer Slider는 Avada token 등록 후 사용 가능함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://themeforest.net/page/top_sellers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. themeforest에서 테마 구매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 구매 후 메뉴 상단의 ID 드롭다운 menu의 Download를 선택하면 아래와 같은 화면이 나옴.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Download 버튼을 선택하고, All files &amp; documentation을 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.Download된 압축 파일을 풀어준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada Themes 폴더에 아바다 테마와 차일드 테마가 있음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. WP 외모에서 본테마를 설치 후 비활성화 상태로 둔다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6. WP 외모에서 차일드 테마를 설치 후 활성화 시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">테마의 파일을 수정,변경시 차일드 테마를 사용하며, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추후 테마가 upgrade되더라도 차일드 테마의 수정 사항은 유지가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. 제품등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테마 설치 후, WP side bar menu에 Avada menu가 생성되며, 이를 선택하고 Registration을 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하단의 Generate A Personal Token link를 선택하여, envateAPI create a token 페이지로 이동한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아래의 항목들을 입력 및 선택 후 create Token을 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Token name : 사용자가 임의로 이름 명시 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Permissions needed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>View Your Envato Account Username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Download Your Purchased Items</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List Purchases You’ve Made</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verify Purchases You've Made</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>therms and conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정상적으로 처리시 Success 와 함께 token이 생성된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생성된 token을 copy하여 WP의 Registration에 입력 후 submit 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8. System Status 체크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">WP side-bar menu에서 Plugins을 선택하면, Avada에서 제공되는 Plugin이 list-up되며, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이를 모두 설치한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9. Avada에서 제공하는 Plug-In 설치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada가 최적화 해 놓은 Plugin이므로, 동일 기능의 Plugin인 경우에는 Avada에서 제공하는 plugin을 사용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10. 테마 patch 하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WP side-bar menu에서 Fusion Patcher를 선택하고, 순서에 맞춰 Patch 실행함.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11. WP의 알림판 &gt; 업데이트 메뉴에서 theme와 Plugin을 update한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada 설치 방법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. sidebar menu 생성 방법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fusion Builder -&gt; Library -&gt; Demos -&gt; Sidebar Page  참조</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Header 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1) Header Content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header의 위치와 Header content의 디자인 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header Position</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top - 7가지 디자인이 있으며, 선택된 디자인에 따른 content를 선택할 수 있다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">슬라이더 설정이 가능한 layout 이며, Header 위/아래 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Left/Right - 한가지 형태이며, Main menu이외의 3개의 content 추가가 가능한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Left</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2) Header Background Image</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 영역에 Background image 설정, image 선택이 없는 경우 background color가 설정됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3) Header Styling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 영역의 Padding(여백) 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 영역 그림자 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo와 Menu 배치를 폭 100%로 사용 - Logo는 좌측, Menu는 우측으로 정렬됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Background color 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sticky Header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 영역에 scroll을 내려도 상단에 유지되도록 하는 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. Logo 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo Alignment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header내의 Logo 위치 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Left</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Center</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 5에서만 사용 가능 - Header layout menu에서 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo Margins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo의 4방향에 대한 margin 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo Background</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Logo의 background color 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lAPnrqeAhAPp0mygCH27vMuMA9XOfIjx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메뉴  한글화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>송장출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마일리지 적립</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QnA - 게시판</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Home 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>템플릿을 기존으로 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sidebar menu가 있는 경우, 100% Width는 설정이 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Side Navi..의 경우, 아래와 같이 메뉴가 하나 더 들어감</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sidebars를 Products Sidebar로 설정 - 포함되는 메뉴는 위젯에서 변경 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heakder Content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content option 4 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Main menu 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada Option - Main menu 높이와 Highlight style 및 color를 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada Option - Menu 정렬 방식 및 Hover color를 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>외모 &gt; Main menu - Sticky 설정을 위해 아래와 같이 설정한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Footer 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Footer widget을 사용하지 않는 경우, OFF로 설정한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Footer widget이 ON되어 있는 상태이며, 목록은 위젯의 Footer Widget 1,2,3,4에서 선택할 수 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sidebar 위젯 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위젯의 Products Sidebar에 woocommerce의 categories를 추가하고, 기존 설정을 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product page의 Sidebar 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada option &gt; Sidebars &gt; Woocommerce Products</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Home을 제외한 모든 Page에 sidebar 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada option &gt; Sidebars &gt; Pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sidebar menu 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Home은 Page내에 별개의 설정이 필요함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada option의 Sidebar의 Pages 설정은 적용되지 않음 - 원인 분석 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product Archive의 Sidebar 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avada option &gt; Sidebars &gt; WooCommerce Archive</t>
+    <t>한글 번역파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Theme-Fusion/Localization-l10n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP  복사 경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">wp-content / languages ​​/ themes </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Woocommerce 한글화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100% 번역된 파일만 WP에서 자동 Update됨. 100%미만은 수동으로 다운로드해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번역파일 생성 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://docs.woocommerce.com/document/woocommerce-localization/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번역파일 경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://translate.wordpress.org/projects/wp-plugins/woocommerce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복사 경로 - WP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wp-contents&gt;languages&gt;plugins</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option의 Sidebar의 Pages 설정보다 각 Page의 sidebar 설정이 우선함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Page sidebar 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada Option에서의 Sidebar 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Page내에서의 Sidebar 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avada option의 sidebar 설정보다 우선적으로 적용된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidebar sticky 설정도 가능함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 page에 option을 일괄 적용하는 방법 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sidebar와 page content간 pading 제거 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://theme-fusion.com/support/documentation/avada-documentation/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mamual</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -519,7 +597,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,6 +694,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -638,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -650,6 +734,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -669,66 +754,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>84896</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>109332</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>584751</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>146914</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="772353" y="8184875"/>
-          <a:ext cx="5278920" cy="3764756"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1185,7 +1210,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1518,7 +1543,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1578,7 +1603,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2894,7 +2919,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3064,7 +3089,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3455,14 +3480,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>156</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>60377</xdr:rowOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>60376</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3510,13 +3535,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>273326</xdr:colOff>
-      <xdr:row>173</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>124240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>339587</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>104332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3565,13 +3590,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>135261</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>115956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>670892</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>150553</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3671,28 +3696,33 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>99390</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>49697</xdr:rowOff>
+      <xdr:colOff>74543</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>289892</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>194014</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>93428</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="그림 30"/>
+        <xdr:cNvPr id="14" name="그림 13"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3706,63 +3736,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1018760" y="24897523"/>
-          <a:ext cx="5466523" cy="3457361"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>74543</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>49696</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>289892</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>93427</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="그림 32"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="993913" y="21170348"/>
-          <a:ext cx="5491370" cy="3149710"/>
+          <a:off x="988943" y="21633346"/>
+          <a:ext cx="5473149" cy="3186981"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3785,24 +3760,24 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>41414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>629480</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>134857</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="그림 34"/>
+        <xdr:cNvPr id="15" name="그림 14"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3816,8 +3791,118 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="927653" y="29237610"/>
-          <a:ext cx="5897218" cy="2164095"/>
+          <a:off x="922683" y="29587964"/>
+          <a:ext cx="5878997" cy="2188943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57980</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>16564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>311663</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="그림 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="977350" y="4571999"/>
+          <a:ext cx="5529704" cy="3486979"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107676</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>51896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>588066</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>137251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="720589" y="11647548"/>
+          <a:ext cx="7437781" cy="3398399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4269,7 +4354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4304,7 +4389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4513,10 +4598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C39"/>
+  <dimension ref="B1:D35"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4528,68 +4613,151 @@
     <col min="5" max="5" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
-        <v>2</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19"/>
+      <c r="D19" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+      <c r="C20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21"/>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27"/>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28"/>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29"/>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30"/>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31"/>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="D17" r:id="rId3"/>
+    <hyperlink ref="D19" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -4611,140 +4779,140 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C32" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C36" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C37" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C39" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C54" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C55" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D56" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E59" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C63" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C64" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J64" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C66" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C67" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
@@ -4768,7 +4936,7 @@
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
       <c r="C76" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D76" s="7"/>
     </row>
@@ -4776,65 +4944,65 @@
       <c r="B77" s="2"/>
       <c r="C77" s="9"/>
       <c r="D77" s="7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
       <c r="C78" s="9"/>
       <c r="D78" s="7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
       <c r="C79" s="9"/>
       <c r="D79" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
       <c r="C80" s="9"/>
       <c r="D80" s="7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C81"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C83" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C84" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B96" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B98" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -4870,62 +5038,62 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D18" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D19" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D20" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D21" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E22" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D23" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D26" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
@@ -4933,12 +5101,12 @@
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4970,12 +5138,12 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -5003,92 +5171,92 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F81" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F93" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C107" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D108" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C134" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D135" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="144" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D144" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="184" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D184" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="185" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E185" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5119,57 +5287,57 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D32" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D39" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -5185,10 +5353,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D169"/>
+  <dimension ref="B2:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A136" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="Q149" sqref="Q149"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A115" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="D100" sqref="C100:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5200,136 +5368,92 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D84" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C101" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C102" s="2"/>
-      <c r="D102" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C103" s="2"/>
-      <c r="D103" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C120" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C121" s="2"/>
-      <c r="D121" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C140" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C141" s="2"/>
-      <c r="D141" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B155" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C156" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C169" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C115" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -5342,10 +5466,96 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D56"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A58" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="4" style="2" customWidth="1"/>
+    <col min="3" max="9" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+      <c r="D41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[Avada] classic shop demo setup #3
</commit_message>
<xml_diff>
--- a/WP themes_Avada review data.xlsx
+++ b/WP themes_Avada review data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="basic Inform" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'WP Reset'!$A$1:$M$67</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">상품page!$A$1:$Q$96</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>max_execution_time 180</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -590,6 +590,18 @@
   </si>
   <si>
     <t>mamual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우커머스 상품페이지에 notice를 별개의 content로 추가하는 방법 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우커머스 상품페이지 layout 설정 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://cafe.naver.com/wphome/67766</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4354,7 +4366,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4389,7 +4401,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4598,10 +4610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D35"/>
+  <dimension ref="B1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4736,14 +4748,29 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4755,9 +4782,10 @@
     <hyperlink ref="D19" r:id="rId4"/>
     <hyperlink ref="D7" r:id="rId5"/>
     <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="B41" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId7"/>
+  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="4294967292" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>